<commit_message>
Update BOM to reflect newly found better components
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68dd1fbc4a1fec30/BVE Controller/r68-bve-mascon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{19E8F56B-3956-4FD0-A5A4-3F8D3960DA8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{45BD1411-0376-4AF0-8896-DF361FCB8F3B}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{19E8F56B-3956-4FD0-A5A4-3F8D3960DA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA9BEA7-B3AD-4DD9-83B9-49D226F87F58}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8DEAC2B2-0883-432A-AA6A-E7B48A9E3554}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8DEAC2B2-0883-432A-AA6A-E7B48A9E3554}"/>
   </bookViews>
   <sheets>
     <sheet name="Definite BOM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Sonar Sensor</t>
   </si>
@@ -97,22 +97,31 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Secure case ends</t>
-  </si>
-  <si>
-    <t>1/4" dia Aluminum Rod</t>
-  </si>
-  <si>
-    <t>https://www.lowes.com/pd/Hillman-1-4-in-dia-x-3-ft-L-Mill-Finished-Aluminum-Solid-Round-Rod/3053649</t>
-  </si>
-  <si>
-    <t>3/4" dia PVC Pipe</t>
-  </si>
-  <si>
-    <t>Secure handle</t>
-  </si>
-  <si>
-    <t>https://www.lowes.com/pd/Charlotte-Pipe-3-4-in-dia-x-10-ft-L-480-PSI-PVC-Pipe/3133085</t>
+    <t>Sparkfun Qwiic Pro Micro</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>https://www.microcenter.com/product/621833/sparkfun-electronics-qwiic-pro-micro-usb-c-(atmega32u4)</t>
+  </si>
+  <si>
+    <t>Can be substituted for any Arduino Pro Micro or anything with an Atmega32U4 for HID support</t>
+  </si>
+  <si>
+    <t>Wire Limit Switch</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07T4SYVYG/</t>
+  </si>
+  <si>
+    <t>Stranded Wire</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" activeCellId="1" sqref="A4:E4 A7:E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,20 +587,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17A1D6-D8E8-4F70-9881-346A9BF19F43}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -599,13 +608,16 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -613,57 +625,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
+        <v>26</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new items to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68dd1fbc4a1fec30/BVE Controller/r68-bve-mascon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{19E8F56B-3956-4FD0-A5A4-3F8D3960DA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA9BEA7-B3AD-4DD9-83B9-49D226F87F58}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{19E8F56B-3956-4FD0-A5A4-3F8D3960DA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBC29A38-1C0F-4F2C-8EE0-585E79A6E255}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8DEAC2B2-0883-432A-AA6A-E7B48A9E3554}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Sonar Sensor</t>
   </si>
@@ -97,24 +97,12 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Sparkfun Qwiic Pro Micro</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Microcontroller</t>
-  </si>
-  <si>
-    <t>https://www.microcenter.com/product/621833/sparkfun-electronics-qwiic-pro-micro-usb-c-(atmega32u4)</t>
-  </si>
-  <si>
-    <t>Can be substituted for any Arduino Pro Micro or anything with an Atmega32U4 for HID support</t>
-  </si>
-  <si>
     <t>Wire Limit Switch</t>
   </si>
   <si>
@@ -122,16 +110,42 @@
   </si>
   <si>
     <t>Stranded Wire</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08C5CTNZR/</t>
+  </si>
+  <si>
+    <t>Cam Follower</t>
+  </si>
+  <si>
+    <t>Notch Detents</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07C5NPXMZ/</t>
+  </si>
+  <si>
+    <t>Ball Bearings Mounted</t>
+  </si>
+  <si>
+    <t>Bearing support on wall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,13 +168,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,17 +604,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17A1D6-D8E8-4F70-9881-346A9BF19F43}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,10 +628,10 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,37 +644,51 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{92B856A6-494E-428D-A20A-02032941FD4E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>